<commit_message>
combined dataframes from years 2016-2021
</commit_message>
<xml_diff>
--- a/ACS_population_Tableau.xlsx
+++ b/ACS_population_Tableau.xlsx
@@ -1,99 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jenkir\Desktop\BDC\Baltimore_Together\measuring-success-metrics\analysis_nbs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{849BD51E-1202-42AB-8BB2-DBAAA62B9607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Households with one or more people under 18 years</t>
-  </si>
-  <si>
-    <t>Total households</t>
-  </si>
-  <si>
-    <t>Population</t>
-  </si>
-  <si>
-    <t>Median age</t>
-  </si>
-  <si>
-    <t>Pop. white</t>
-  </si>
-  <si>
-    <t>Pop. Black</t>
-  </si>
-  <si>
-    <t>Pop. Hispanic origin</t>
-  </si>
-  <si>
-    <t>Pop. &lt;18 years</t>
-  </si>
-  <si>
-    <t>Pop. working age</t>
-  </si>
-  <si>
-    <t>Pop. 65+ years</t>
-  </si>
-  <si>
-    <t>Percent working age</t>
-  </si>
-  <si>
-    <t>Percent households with children</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2018</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2021</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,53 +46,93 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -442,277 +420,300 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="14.88671875" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.77734375" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.44140625" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="13.21875" customWidth="1"/>
-    <col min="12" max="12" width="13.44140625" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Households with one or more people under 18 years</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total households</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Population</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Median age</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Pop. white</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Pop. Black</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Pop. Hispanic origin</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Pop. &lt;18 years</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Pop. working age</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Pop. 65+ years</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Percent working age</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Percent households with children</t>
+        </is>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2016</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>59079</v>
+      </c>
+      <c r="C2" t="n">
+        <v>240761</v>
+      </c>
+      <c r="D2" t="n">
+        <v>614664</v>
+      </c>
+      <c r="E2" t="n">
+        <v>34.9</v>
+      </c>
+      <c r="F2" t="n">
+        <v>189260</v>
+      </c>
+      <c r="G2" t="n">
+        <v>384465</v>
+      </c>
+      <c r="H2" t="n">
+        <v>31144</v>
+      </c>
+      <c r="I2" t="n">
+        <v>129154</v>
+      </c>
+      <c r="J2" t="n">
+        <v>406262</v>
+      </c>
+      <c r="K2" t="n">
+        <v>79248</v>
+      </c>
+      <c r="L2" t="n">
+        <v>66</v>
+      </c>
+      <c r="M2" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2017</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>59831</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" t="n">
         <v>240280</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D3" t="n">
         <v>611648</v>
       </c>
-      <c r="E2" s="5">
-        <v>35.299999999999997</v>
-      </c>
-      <c r="F2" s="5">
+      <c r="E3" t="n">
+        <v>35.3</v>
+      </c>
+      <c r="F3" t="n">
         <v>183988</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G3" t="n">
         <v>383508</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H3" t="n">
         <v>32495</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I3" t="n">
         <v>126007</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J3" t="n">
         <v>403089</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K3" t="n">
         <v>82552</v>
       </c>
-      <c r="L2" s="5">
+      <c r="L3" t="n">
         <v>65</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M3" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2018</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
         <v>55371</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C4" t="n">
         <v>237204</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D4" t="n">
         <v>602495</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E4" t="n">
         <v>35.5</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F4" t="n">
         <v>183276</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G4" t="n">
         <v>371664</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H4" t="n">
         <v>33061</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I4" t="n">
         <v>123114</v>
       </c>
-      <c r="J3" s="5">
+      <c r="J4" t="n">
         <v>395312</v>
       </c>
-      <c r="K3" s="5">
+      <c r="K4" t="n">
         <v>84069</v>
       </c>
-      <c r="L3" s="5">
+      <c r="L4" t="n">
         <v>65</v>
       </c>
-      <c r="M3" s="5">
+      <c r="M4" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="5">
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2019</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>58250</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" t="n">
         <v>242694</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D5" t="n">
         <v>593490</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E5" t="n">
         <v>35.9</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F5" t="n">
         <v>179979</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G5" t="n">
         <v>371243</v>
       </c>
-      <c r="H4" s="5">
+      <c r="H5" t="n">
         <v>33652</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I5" t="n">
         <v>119567</v>
       </c>
-      <c r="J4" s="5">
+      <c r="J5" t="n">
         <v>387658</v>
       </c>
-      <c r="K4" s="5">
+      <c r="K5" t="n">
         <v>86265</v>
       </c>
-      <c r="L4" s="5">
+      <c r="L5" t="n">
         <v>65</v>
       </c>
-      <c r="M4" s="5">
+      <c r="M5" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="5">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> 2021</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>55571</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6" t="n">
         <v>254370</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D6" t="n">
         <v>576498</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E6" t="n">
         <v>36.1</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F6" t="n">
         <v>159246</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G6" t="n">
         <v>344531</v>
       </c>
-      <c r="H5" s="5">
+      <c r="H6" t="n">
         <v>34810</v>
       </c>
-      <c r="I5" s="5">
+      <c r="I6" t="n">
         <v>116862</v>
       </c>
-      <c r="J5" s="5">
+      <c r="J6" t="n">
         <v>374406</v>
       </c>
-      <c r="K5" s="5">
+      <c r="K6" t="n">
         <v>85230</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L6" t="n">
         <v>64</v>
       </c>
-      <c r="M5" s="5">
+      <c r="M6" t="n">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5"/>
-      <c r="L6" s="5"/>
-      <c r="M6" s="5"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
-      <c r="M7" s="5"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>